<commit_message>
add button infobulle, remove button titles
</commit_message>
<xml_diff>
--- a/WebAppMobility/nomenclature.xlsx
+++ b/WebAppMobility/nomenclature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/21ac13b765b5810b/Documents/ING2/PDI19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{BAEF8442-C649-43C0-B263-F38037E46BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70329527-60B3-4081-ABAF-E7BE00AB07DD}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{BAEF8442-C649-43C0-B263-F38037E46BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98440144-DE5E-47C9-983B-00142C71A002}"/>
   <bookViews>
     <workbookView xWindow="10178" yWindow="0" windowWidth="10425" windowHeight="13043" xr2:uid="{A7CE64EE-2919-41C9-9151-682E899E7B4F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="98">
   <si>
     <t>id</t>
   </si>
@@ -129,12 +129,6 @@
     <t>sim_button</t>
   </si>
   <si>
-    <t>title_download_csv</t>
-  </si>
-  <si>
-    <t>title_launch</t>
-  </si>
-  <si>
     <t>button dl csv</t>
   </si>
   <si>
@@ -144,9 +138,6 @@
     <t>button dl svg</t>
   </si>
   <si>
-    <t>title_download_svg</t>
-  </si>
-  <si>
     <t>graph</t>
   </si>
   <si>
@@ -162,18 +153,6 @@
     <t>settings</t>
   </si>
   <si>
-    <t>title button settings</t>
-  </si>
-  <si>
-    <t>title_settings</t>
-  </si>
-  <si>
-    <t>title button dl csv</t>
-  </si>
-  <si>
-    <t>title button launch</t>
-  </si>
-  <si>
     <t>choice csp</t>
   </si>
   <si>
@@ -277,6 +256,78 @@
   </si>
   <si>
     <t>infobulle8</t>
+  </si>
+  <si>
+    <t>infobulle</t>
+  </si>
+  <si>
+    <t>dl_CSV</t>
+  </si>
+  <si>
+    <t>dl_SVG</t>
+  </si>
+  <si>
+    <t>global_container</t>
+  </si>
+  <si>
+    <t>global container</t>
+  </si>
+  <si>
+    <t>div_mobility</t>
+  </si>
+  <si>
+    <t>box mobility</t>
+  </si>
+  <si>
+    <t>button infobulle</t>
+  </si>
+  <si>
+    <t>b_infobulle1</t>
+  </si>
+  <si>
+    <t>button_infobulle</t>
+  </si>
+  <si>
+    <t>b_infobulle2</t>
+  </si>
+  <si>
+    <t>button infobulle2</t>
+  </si>
+  <si>
+    <t>button infobulle3</t>
+  </si>
+  <si>
+    <t>b_infobulle3</t>
+  </si>
+  <si>
+    <t>button infobulle4</t>
+  </si>
+  <si>
+    <t>b_infobulle4</t>
+  </si>
+  <si>
+    <t>button infobulle5</t>
+  </si>
+  <si>
+    <t>b_infobulle5</t>
+  </si>
+  <si>
+    <t>button infobulle6</t>
+  </si>
+  <si>
+    <t>b_infobulle6</t>
+  </si>
+  <si>
+    <t>button infobulle7</t>
+  </si>
+  <si>
+    <t>b_infobulle7</t>
+  </si>
+  <si>
+    <t>button infobulle8</t>
+  </si>
+  <si>
+    <t>b_infobulle8</t>
   </si>
 </sst>
 </file>
@@ -318,24 +369,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -370,10 +408,12 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -382,12 +422,12 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,137 +742,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E9CE7D-E470-4144-8F55-68E420D2BB09}">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="18.59765625" customWidth="1"/>
     <col min="2" max="2" width="22.9296875" customWidth="1"/>
-    <col min="3" max="3" width="11.53125" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="6"/>
+      <c r="A2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="C4" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="A9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>72</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>7</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="1"/>
+        <v>84</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="2"/>
@@ -841,19 +885,21 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>7</v>
@@ -861,25 +907,33 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="A18" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C19" s="1" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
@@ -889,52 +943,54 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B22" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C22" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="1"/>
+        <v>89</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B24" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="C24" s="1" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="1"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
@@ -942,91 +998,93 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A27" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" s="1"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="1"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+      <c r="A29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" s="1"/>
+        <v>91</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="C31" s="1" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="1"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C35" s="1"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
@@ -1036,16 +1094,16 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="C38" s="1"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
@@ -1054,169 +1112,195 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40" s="1"/>
+        <v>93</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B41" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C41" s="1" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B42" s="1"/>
       <c r="C42" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" s="1"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
+      <c r="A44" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>26</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A46" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>80</v>
+        <v>21</v>
       </c>
       <c r="C47" s="1"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C48" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
+      <c r="A49" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>76</v>
+        <v>25</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C50" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C51" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
+      <c r="A52" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A54" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C54" s="1"/>
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
+      <c r="A55" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B56" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="C56" s="1" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C57" s="1"/>
+        <v>97</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
+      <c r="A58" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A59" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C59" s="4"/>
+      <c r="A59" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C59" s="1"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A60" s="2"/>
@@ -1225,21 +1309,52 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C61" s="1"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A62" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C62" s="3"/>
+      <c r="A62" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A63" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A64" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C64" s="4"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A65" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C65" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>